<commit_message>
Actually added the .db file
</commit_message>
<xml_diff>
--- a/SampleData/SampleData.xlsx
+++ b/SampleData/SampleData.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpnor\Documents\GitHub\Project-SERVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpnor\Documents\GitHub\Project-SERVE\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDBE1736-C89C-479C-BF70-32A58C10560D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB5135-270E-462A-8907-566CB7172845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="7" activeTab="12" xr2:uid="{6E194161-9C50-4581-8B8F-BB9EE36C3AE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="9" activeTab="12" xr2:uid="{6E194161-9C50-4581-8B8F-BB9EE36C3AE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Executives" sheetId="2" r:id="rId1"/>
-    <sheet name="Student" sheetId="3" r:id="rId2"/>
+    <sheet name="Member" sheetId="3" r:id="rId2"/>
     <sheet name="Term" sheetId="4" r:id="rId3"/>
     <sheet name="Session" sheetId="5" r:id="rId4"/>
     <sheet name="Tournament" sheetId="6" r:id="rId5"/>
     <sheet name="Team" sheetId="7" r:id="rId6"/>
     <sheet name="Account" sheetId="8" r:id="rId7"/>
-    <sheet name="Member-Valid_For-Term" sheetId="9" r:id="rId8"/>
-    <sheet name="Executive-For-Term" sheetId="10" r:id="rId9"/>
-    <sheet name="Member-Attend-Session" sheetId="11" r:id="rId10"/>
-    <sheet name="Member-Make-Team" sheetId="12" r:id="rId11"/>
+    <sheet name="Member_Valid_For_Term" sheetId="9" r:id="rId8"/>
+    <sheet name="Executive_For_Term" sheetId="10" r:id="rId9"/>
+    <sheet name="Member_Attend_Session" sheetId="11" r:id="rId10"/>
+    <sheet name="Member_Make_Team" sheetId="12" r:id="rId11"/>
     <sheet name="Session_Levels" sheetId="13" r:id="rId12"/>
     <sheet name="Tournament_Levels" sheetId="14" r:id="rId13"/>
   </sheets>
@@ -405,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,14 +415,13 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -786,7 +785,7 @@
       <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E1" t="s">
@@ -877,10 +876,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1004,10 +1003,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1059,10 +1058,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1130,10 +1129,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1176,7 +1175,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B52AE39-5C1E-41FF-9BEE-440A3A7892D2}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
@@ -1194,7 +1193,7 @@
       <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E1" t="s">
@@ -1405,10 +1404,10 @@
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>2</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1431,7 +1430,7 @@
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>3</v>
       </c>
       <c r="H10" s="4" t="s">
@@ -1458,111 +1457,108 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{9451D62C-F22E-4B95-A67E-E3E5D168A816}"/>
@@ -1589,7 +1585,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B1" t="s">
@@ -1637,7 +1633,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
@@ -1663,10 +1659,10 @@
       <c r="B2" s="1">
         <v>45452</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>0.89583333333333337</v>
       </c>
       <c r="E2" t="s">
@@ -1683,10 +1679,10 @@
       <c r="B3" s="1">
         <v>45482</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>0.5</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>0.54166666666666663</v>
       </c>
       <c r="E3" t="s">
@@ -1715,7 +1711,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
@@ -1747,10 +1743,10 @@
       <c r="B2" s="1">
         <v>45454</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>0.91666666666666663</v>
       </c>
       <c r="E2" t="s">
@@ -1780,7 +1776,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B1" t="s">
@@ -1840,7 +1836,7 @@
       <c r="A1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1876,10 +1872,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1996,10 +1992,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C1" t="s">

</xml_diff>

<commit_message>
deleted unnecessary serve, changed some title formatting
</commit_message>
<xml_diff>
--- a/SampleData/SampleData.xlsx
+++ b/SampleData/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpnor\Documents\GitHub\Project-SERVE\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AB5135-270E-462A-8907-566CB7172845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F4ACD3-98C6-49F7-88CB-68E325B99B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="9" activeTab="12" xr2:uid="{6E194161-9C50-4581-8B8F-BB9EE36C3AE1}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" firstSheet="8" activeTab="8" xr2:uid="{6E194161-9C50-4581-8B8F-BB9EE36C3AE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Executives" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Team" sheetId="7" r:id="rId6"/>
     <sheet name="Account" sheetId="8" r:id="rId7"/>
     <sheet name="Member_Valid_For_Term" sheetId="9" r:id="rId8"/>
-    <sheet name="Executive_For_Term" sheetId="10" r:id="rId9"/>
+    <sheet name="Executive_Works_For_Term" sheetId="10" r:id="rId9"/>
     <sheet name="Member_Attend_Session" sheetId="11" r:id="rId10"/>
     <sheet name="Member_Make_Team" sheetId="12" r:id="rId11"/>
     <sheet name="Session_Levels" sheetId="13" r:id="rId12"/>
@@ -773,9 +773,9 @@
       <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>20943819</v>
       </c>
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>98765432</v>
       </c>
@@ -835,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>19283746</v>
       </c>
@@ -873,9 +873,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -883,7 +883,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -891,7 +891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -899,7 +899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -907,7 +907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -923,7 +923,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -931,7 +931,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -939,7 +939,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -947,7 +947,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -955,7 +955,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>35</v>
       </c>
@@ -963,7 +963,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -971,7 +971,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -979,7 +979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1000,9 +1000,9 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1055,9 +1055,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1122,13 +1122,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE15ADD-2F5F-4D92-8AC1-523787704F8F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1181,9 +1181,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>21017215</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>21012631</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>20905813</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>21010674</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>21067881</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>21111453</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>12345678</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>20943292</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>21001713</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>21001714</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1474,7 +1474,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1491,7 +1491,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1508,7 +1508,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1525,7 +1525,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1542,7 +1542,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1582,9 +1582,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1630,9 +1630,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1705,12 +1705,12 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1773,9 +1773,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>75</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -1830,9 +1830,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="51" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>83</v>
       </c>
@@ -1869,9 +1869,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -1985,13 +1985,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5AB4CC2-881D-48BC-9D41-C126B0142A45}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>

</xml_diff>